<commit_message>
Fixes needed. Use new-formtunnel to test
</commit_message>
<xml_diff>
--- a/docs/AdminToolbox.FortiWizard/Examples/VPN Buildout Form.xlsx
+++ b/docs/AdminToolbox.FortiWizard/Examples/VPN Buildout Form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Github\AdminToolbox\docs\AdminToolbox.FortiWizard\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F5742D-5771-42CA-8E4B-9469313DDE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF303682-6E73-40E7-946D-50BA13F6D79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="405" windowWidth="29040" windowHeight="15195" xr2:uid="{5549AC1C-0D2B-4CC9-98FF-5DC810AE9CED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{5549AC1C-0D2B-4CC9-98FF-5DC810AE9CED}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -100,9 +100,6 @@
     <t>wan</t>
   </si>
   <si>
-    <t>port2</t>
-  </si>
-  <si>
     <t>192.168.10.0/24, 192.168.11.0/24, 192.168.12.0/24</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
   </si>
   <si>
     <t>1.1.1.1</t>
-  </si>
-  <si>
-    <t>aes256-sha512</t>
   </si>
   <si>
     <t>fgbGF^&amp;745fgokm</t>
@@ -489,6 +483,12 @@
   </si>
   <si>
     <t>LAN Interface</t>
+  </si>
+  <si>
+    <t>port1, voice vlan</t>
+  </si>
+  <si>
+    <t>aes256-sha512, aes128-sha256</t>
   </si>
 </sst>
 </file>
@@ -612,6 +612,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -636,15 +640,11 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1089,118 +1089,118 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467F2439-AFA4-4EB5-9722-C78966753CCE}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L1" sqref="L1:X1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-    </row>
-    <row r="2" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+    </row>
+    <row r="2" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-    </row>
-    <row r="3" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+    </row>
+    <row r="3" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-    </row>
-    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+    </row>
+    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
       <c r="F6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
       <c r="F7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
       <c r="F8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
       <c r="K8" s="2"/>
     </row>
   </sheetData>
@@ -1227,300 +1227,294 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E6"/>
+      <selection activeCell="B11" sqref="B11:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="17" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-    </row>
-    <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="17" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+    </row>
+    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-    </row>
-    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+    </row>
+    <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="17" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="18">
         <v>22800</v>
       </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="18">
+        <v>2</v>
+      </c>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16">
-        <v>2</v>
-      </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="F17:J17"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="F13:J13"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="F7:J7"/>
     <mergeCell ref="F10:J10"/>
@@ -1537,14 +1531,20 @@
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B8:E8"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B15:E15"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:J14"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="F15:J15"/>
   </mergeCells>
   <dataValidations count="10">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Length" error="Tunnel Name must be less than 15 characters." promptTitle="Tunnel Name" prompt="This will be the name of the tunnel built on our Firewall. Must be less than 15 characters." sqref="B6:E6" xr:uid="{03F195E0-AFC6-4FC7-8F1F-7DE63D349659}">
@@ -1553,7 +1553,7 @@
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Peer Address" prompt="This is the public IP for our side of the tunnel." sqref="B5:E5" xr:uid="{B1CD10FA-442D-4821-B42B-4B39A66D9E15}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Local CIDRS" prompt="These are the subnets or hosts included for our side of the tunnel. Enter in comma delimited format." sqref="B4:E4" xr:uid="{4BF649B0-944E-4A20-8E77-1A3D709EDDA8}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="LAN Interface" prompt="This is the LAN interface for our side of the tunnel and the input is case sensitive." sqref="B3:E3" xr:uid="{C4ABC9DB-F48D-4A25-9FEE-2D172D88EAE1}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="LAN Interface" prompt="This is the LAN interface or interfaces for our side of the tunnel. Input is case sensitive." sqref="B3:E3" xr:uid="{C4ABC9DB-F48D-4A25-9FEE-2D172D88EAE1}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Wan Interface" prompt="This is the WAN interface for our side of the tunnel and the input is case sensitive." sqref="B2:E2" xr:uid="{5B209772-0939-489C-9330-2A4A4C0FD6A4}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Subnets or Hosts" prompt="These are the subnets included for your side of the tunnel. Enter in comma delimited format as shown in the example." sqref="B8:E8" xr:uid="{F3FC9BFB-1638-4D1D-B294-12AA2CC89311}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Public IP" prompt="This is the public IP for your side of the tunnel." sqref="B9:E9" xr:uid="{90ECDB5C-D46F-431F-82F5-D71ABBC94518}"/>
@@ -1568,7 +1568,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value Check" error="The value you entered doesn't match an option from the dropdown menu. Please use the drop down menu to select an option." promptTitle="Select an Option" prompt="Select a valid Phase 1 and Phase 2 proposal option from the drop down menu." xr:uid="{309CAFB7-A57D-4A82-9EF5-6DF84A1237ED}">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value Check" error="The value you entered doesn't match an option from the dropdown menu. Please use the drop down menu to select an option or ensure the format entered matches the example." promptTitle="Select an Option" prompt="Select a valid Phase 1 and Phase 2 proposal option from the drop down menu. If multiple values, they can be entered using the format shown in the example." xr:uid="{309CAFB7-A57D-4A82-9EF5-6DF84A1237ED}">
           <x14:formula1>
             <xm:f>'Data Validation'!$A$2:$A$26</xm:f>
           </x14:formula1>
@@ -1603,304 +1603,324 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:E18"/>
+      <selection activeCell="B12" sqref="B12:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="13.85546875" customWidth="1"/>
+    <col min="1" max="5" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="17" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-    </row>
-    <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="17" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+    </row>
+    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-    </row>
-    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+    </row>
+    <row r="11" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="17" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="16">
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="18">
         <v>22800</v>
       </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="18">
+        <v>2</v>
+      </c>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="16">
-        <v>2</v>
-      </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="F8:J8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:J9"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="F17:J17"/>
     <mergeCell ref="B18:E18"/>
@@ -1917,26 +1937,6 @@
     <mergeCell ref="F12:J12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="F13:J13"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="F8:J8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:J9"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:J6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:J2"/>
   </mergeCells>
   <dataValidations count="11">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Local CIDRS" prompt="These are the NAT subnets or hosts included for our side of the tunnel. Enter in comma delimited format." sqref="B5:E5" xr:uid="{62A4F800-5137-4B7F-A2F4-0F3093E623BD}"/>
@@ -1946,7 +1946,6 @@
       <formula2>14</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Local CIDRS" prompt="These are the subnets or hosts included for our side of the tunnel. Enter in comma delimited format." sqref="B4:E4" xr:uid="{E30D207E-969F-4389-83B6-6C97BDCA84CC}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="LAN Interface" prompt="This is the LAN interface for our side of the tunnel and the input is case sensitive." sqref="B3:E3" xr:uid="{03ED220E-B2B3-4D77-94F9-2B68C85D84C7}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Wan Interface" prompt="This is the WAN interface for our side of the tunnel and the input is case sensitive." sqref="B2:E2" xr:uid="{BA9BED3D-FC45-4642-99A7-C3D1037C4C1E}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Public IP" prompt="This is the public IP for your side of the tunnel." sqref="B10:E10" xr:uid="{E1D19247-04BB-4443-99DE-0A2763CE91C9}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Subnets or Hosts" prompt="These are the subnets included for your side of the tunnel. Enter in comma delimited format as shown in the example." sqref="B9:E9" xr:uid="{26978246-CC60-409C-8F88-3E819C638BC1}"/>
@@ -1956,6 +1955,7 @@
       <formula2>86400</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Leave Blank if All" prompt="These are the services that will be allowed for the tunnel. They should be provided in comma delimited format and typed like so… ServiceName/PortRange/Protocol" sqref="B16:E16" xr:uid="{2FFFEDB4-BC71-415C-9EF4-11B51AD3DDD8}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="LAN Interface" prompt="This is the LAN interface or interfaces for our side of the tunnel. Input is case sensitive." sqref="B3:E3" xr:uid="{89AEF286-24FB-481D-9A83-43AFECCB6898}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1979,7 +1979,7 @@
           </x14:formula1>
           <xm:sqref>B15:E15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value Check" error="The value you entered doesn't match an option from the dropdown menu. Please use the drop down menu to select an option." promptTitle="Select an Option" prompt="Select a valid Phase 1 and Phase 2 proposal option from the drop down menu." xr:uid="{4B617EE0-4F6F-4F61-A3AE-FB500283A9B2}">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value Check" error="The value you entered doesn't match an option from the dropdown menu. Please use the drop down menu to select an option or ensure the format entered matches the example." promptTitle="Select an Option" prompt="Select a valid Phase 1 and Phase 2 proposal option from the drop down menu. If multiple values, they can be entered using the format shown in the example." xr:uid="{5CC1424D-68FD-4BAB-865B-3F69AC0D8E5E}">
           <x14:formula1>
             <xm:f>'Data Validation'!$A$2:$A$26</xm:f>
           </x14:formula1>
@@ -1995,290 +1995,312 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A920662-2A14-4585-A258-D7BC09CFE950}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="10" width="11.5703125" customWidth="1"/>
+    <col min="1" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="10" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="17" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-    </row>
-    <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="17" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+    </row>
+    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-    </row>
-    <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="17" t="s">
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="16">
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="18">
         <v>22800</v>
       </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="16" t="s">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="18">
+        <v>187</v>
+      </c>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="18">
+        <v>2</v>
+      </c>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="16">
-        <v>187</v>
-      </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16">
-        <v>2</v>
-      </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:J8"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="F16:J16"/>
     <mergeCell ref="B17:E17"/>
@@ -2291,32 +2313,9 @@
     <mergeCell ref="F12:J12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="F13:J13"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="F9:J9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:J8"/>
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:J6"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <dataValidations count="10">
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Wan Interface" prompt="This is the WAN interface for our side of the tunnel and the input is case sensitive." sqref="B2:E2" xr:uid="{C07FD6AA-6C71-4C27-87CC-503A8E3B46BD}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="LAN Interface" prompt="This is the LAN interface for our side of the tunnel and the input is case sensitive." sqref="B3:E3" xr:uid="{E3AB46DE-BE9E-44DB-801D-F916BE01AE31}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Local CIDRS" prompt="These are the subnets or hosts included for our side of the tunnel. Enter in comma delimited format." sqref="B4:E4" xr:uid="{34119527-BAD6-49DE-A5C0-74EF2DF8CB35}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Peer Address" prompt="This is the public IP for our side of the tunnel." sqref="B5:E5" xr:uid="{C5D5A1BF-EB6B-4F8F-B69D-CA62D29A2644}"/>
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Length" error="Tunnel Name must be less than 15 characters." promptTitle="Tunnel Name" prompt="This will be the name of the tunnel built on our Firewall. Must be less than 15 characters." sqref="B6:E6" xr:uid="{06142386-628E-433F-9F50-3ACDB31310A6}">
@@ -2331,18 +2330,13 @@
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Shared Key" prompt="Please input a private key to be used for the Phase 1 and Phase 2 if pfs is enabled." sqref="B11:E11" xr:uid="{72A00610-33B7-4187-B3A4-884D1FB4B0E4}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Peer ID" prompt="This is a unique 3 numeric character long Identifer for this tunnel.   " sqref="B15:E15" xr:uid="{D15BF637-3655-4D1A-A8C4-1B015D6EF7A7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="LAN Interface" prompt="This is the LAN interface or interfaces for our side of the tunnel. Input is case sensitive." sqref="B3:E3" xr:uid="{E3189C81-B086-4599-B81D-D3C775E08099}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value Check" error="The value you entered doesn't match an option from the dropdown menu. Please use the drop down menu to select an option." promptTitle="Select an Option" prompt="Select a valid Phase 1 and Phase 2 proposal option from the drop down menu." xr:uid="{7CD228D7-7013-4229-AD6E-E62E47DDD9B6}">
-          <x14:formula1>
-            <xm:f>'Data Validation'!$A$2:$A$26</xm:f>
-          </x14:formula1>
-          <xm:sqref>B10:E10</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value Check" error="The value you entered doesn't match an option from the dropdown menu. Please correct or continue if your value matches the format shown in the example." promptTitle="Select an Option" prompt="Select a valid Diffie Hellman Group from the drop down menu, or type your own comma delimited option. Like what is shown in the example." xr:uid="{6FEE91C3-ABD3-43A0-8E18-2C7C180C143B}">
           <x14:formula1>
             <xm:f>'Data Validation'!$C$2:$C$18</xm:f>
@@ -2361,6 +2355,12 @@
           </x14:formula1>
           <xm:sqref>B17:E17</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value Check" error="The value you entered doesn't match an option from the dropdown menu. Please use the drop down menu to select an option or ensure the format entered matches the example." promptTitle="Select an Option" prompt="Select a valid Phase 1 and Phase 2 proposal option from the drop down menu. If multiple values, they can be entered using the format shown in the example." xr:uid="{3CBF86B7-F7E9-4106-BFDF-42007AB9EA9D}">
+          <x14:formula1>
+            <xm:f>'Data Validation'!$A$2:$A$26</xm:f>
+          </x14:formula1>
+          <xm:sqref>B10:E10</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -2375,214 +2375,214 @@
       <selection activeCell="A2" sqref="A2:A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
         <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="20">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="10">
         <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G2" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="20">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="10">
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G3" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="10">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="20">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="C6" s="10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="20">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="C7" s="10">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="20">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="C8" s="10">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="20">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="C9" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="20">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="C10" s="10">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="20">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="C11" s="10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="20">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="C12" s="10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="20">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="C13" s="10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="20">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="C14" s="10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="20">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="C15" s="10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="20">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="C16" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="20">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="C17" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="C18" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2607,6 +2607,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B6CAB0F47CC3754797586B7D92E57C5D" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="41d386b8d08e958c99720414287dc6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="27bdd63d-6ee8-4cd4-b819-860a9527756d" xmlns:ns3="891b5dd6-cc48-4739-b022-bf37421cabd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7e57c0ad5350a9654831ddf9bb92c513" ns2:_="" ns3:_="">
     <xsd:import namespace="27bdd63d-6ee8-4cd4-b819-860a9527756d"/>
@@ -2829,12 +2835,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2352FC38-A6D7-4700-A093-3B0BD301C6E7}">
   <ds:schemaRefs>
@@ -2844,6 +2844,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DB187FE-51AC-4561-AC8E-FAFC09F1C9C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F1C8CA7-7272-4C7C-89EE-4682936E3FAD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2860,13 +2869,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DB187FE-51AC-4561-AC8E-FAFC09F1C9C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add Parameters tunnel buildout Fixes #37
</commit_message>
<xml_diff>
--- a/docs/AdminToolbox.FortiWizard/Examples/VPN Buildout Form.xlsx
+++ b/docs/AdminToolbox.FortiWizard/Examples/VPN Buildout Form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Github\AdminToolbox\docs\AdminToolbox.FortiWizard\Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taylo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF303682-6E73-40E7-946D-50BA13F6D79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97E6A2B-8AC9-40CB-AA95-210DA123C7F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{5549AC1C-0D2B-4CC9-98FF-5DC810AE9CED}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{5549AC1C-0D2B-4CC9-98FF-5DC810AE9CED}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="69">
   <si>
     <t>&lt;Company Name&gt; VPN Buildout Form</t>
   </si>
@@ -489,6 +489,12 @@
   </si>
   <si>
     <t>aes256-sha512, aes128-sha256</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Tunnel for product integration</t>
   </si>
 </sst>
 </file>
@@ -634,17 +640,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1093,9 +1099,9 @@
       <selection activeCell="L1" sqref="L1:X1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" ht="25.8" x14ac:dyDescent="0.95">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -1109,7 +1115,7 @@
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
     </row>
-    <row r="2" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -1123,7 +1129,7 @@
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
     </row>
-    <row r="3" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="16" t="s">
         <v>18</v>
       </c>
@@ -1137,7 +1143,7 @@
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
     </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="18.3" x14ac:dyDescent="0.7">
       <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
@@ -1154,7 +1160,7 @@
       <c r="J5" s="15"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1170,7 +1176,7 @@
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1186,7 +1192,7 @@
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1224,20 +1230,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA6D4131-A607-49C7-BE92-430514422210}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.3125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1015625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="10.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.3" x14ac:dyDescent="0.7">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -1245,95 +1251,95 @@
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="18" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="18" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-    </row>
-    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+    </row>
+    <row r="7" spans="1:10" ht="18.3" x14ac:dyDescent="0.7">
       <c r="A7" s="15" t="s">
         <v>22</v>
       </c>
@@ -1341,184 +1347,208 @@
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18" t="s">
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-    </row>
-    <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+    </row>
+    <row r="10" spans="1:10" ht="18.3" x14ac:dyDescent="0.7">
+      <c r="A10" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18" t="s">
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="18">
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="17">
         <v>22800</v>
       </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="18" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="18" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="18">
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="17">
         <v>2</v>
       </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18" t="s">
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="F14:J14"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="F2:J2"/>
+  <mergeCells count="36">
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="F3:J3"/>
     <mergeCell ref="F4:J4"/>
@@ -1531,22 +1561,16 @@
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B8:E8"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="F17:J17"/>
-    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="F2:J2"/>
   </mergeCells>
-  <dataValidations count="10">
+  <dataValidations count="11">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Length" error="Tunnel Name must be less than 15 characters." promptTitle="Tunnel Name" prompt="This will be the name of the tunnel built on our Firewall. Must be less than 15 characters." sqref="B6:E6" xr:uid="{03F195E0-AFC6-4FC7-8F1F-7DE63D349659}">
       <formula1>1</formula1>
       <formula2>14</formula2>
@@ -1563,6 +1587,7 @@
       <formula2>86400</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Shared Key" prompt="Please input a private key to be used for the Phase 1 and Phase 2 if pfs is enabled." sqref="B12:E12" xr:uid="{9E459AD0-C2F6-47D4-82A2-D143255F65EC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Tunnel Description" prompt="Comments are added to the tunnel interface. Useful for quick reminders of a tunnels purpose, or for recording information related to the tunnel." sqref="B18:E18" xr:uid="{DE7C5FA9-B9B7-48B2-A628-948DA318A4DA}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1600,18 +1625,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E09B223A-56BE-4F04-87ED-767E7017E672}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:E12"/>
+      <selection activeCell="A19" sqref="A19:J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="5" width="13.88671875" customWidth="1"/>
+    <col min="1" max="5" width="13.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.3" x14ac:dyDescent="0.7">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -1619,111 +1644,111 @@
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="18" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="18" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="18" t="s">
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-    </row>
-    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+    </row>
+    <row r="8" spans="1:10" ht="18.3" x14ac:dyDescent="0.7">
       <c r="A8" s="15" t="s">
         <v>22</v>
       </c>
@@ -1731,196 +1756,194 @@
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18" t="s">
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="18" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-    </row>
-    <row r="11" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+    </row>
+    <row r="11" spans="1:10" ht="18.3" x14ac:dyDescent="0.7">
+      <c r="A11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="20" t="s">
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18" t="s">
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="18" t="s">
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="18">
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="17">
         <v>22800</v>
       </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="18" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="18" t="s">
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18">
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="17">
         <v>2</v>
       </c>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="18" t="s">
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:J6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="F8:J8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:J9"/>
+  <mergeCells count="38">
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:J19"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="F17:J17"/>
     <mergeCell ref="B18:E18"/>
@@ -1937,8 +1960,28 @@
     <mergeCell ref="F12:J12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="F13:J13"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="F8:J8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:J6"/>
   </mergeCells>
-  <dataValidations count="11">
+  <dataValidations count="12">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Local CIDRS" prompt="These are the NAT subnets or hosts included for our side of the tunnel. Enter in comma delimited format." sqref="B5:E5" xr:uid="{62A4F800-5137-4B7F-A2F4-0F3093E623BD}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Peer Address" prompt="This is the public IP for our side of the tunnel." sqref="B6:E6" xr:uid="{B916A99D-BBBF-4A85-A11F-9FEC21EDD7A5}"/>
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Length" error="Tunnel Name must be less than 15 characters." promptTitle="Tunnel Name" prompt="This will be the name of the tunnel built on our Firewall. Must be less than 15 characters." sqref="B7:E7" xr:uid="{55936FBF-0288-4744-81C2-CC7D0EF86484}">
@@ -1956,6 +1999,7 @@
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Leave Blank if All" prompt="These are the services that will be allowed for the tunnel. They should be provided in comma delimited format and typed like so… ServiceName/PortRange/Protocol" sqref="B16:E16" xr:uid="{2FFFEDB4-BC71-415C-9EF4-11B51AD3DDD8}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="LAN Interface" prompt="This is the LAN interface or interfaces for our side of the tunnel. Input is case sensitive." sqref="B3:E3" xr:uid="{89AEF286-24FB-481D-9A83-43AFECCB6898}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Tunnel Description" prompt="Comments are added to the tunnel interface. Useful for quick reminders of a tunnels purpose, or for recording information related to the tunnel." sqref="B19:E19" xr:uid="{AD40D9B6-954A-480B-9A7C-B25635168820}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1993,19 +2037,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A920662-2A14-4585-A258-D7BC09CFE950}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="A18:J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="10" width="11.5546875" customWidth="1"/>
+    <col min="1" max="5" width="13.68359375" customWidth="1"/>
+    <col min="6" max="10" width="11.5234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.3" x14ac:dyDescent="0.7">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -2013,95 +2057,95 @@
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="18" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="18" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-    </row>
-    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+    </row>
+    <row r="7" spans="1:10" ht="18.3" x14ac:dyDescent="0.7">
       <c r="A7" s="15" t="s">
         <v>22</v>
       </c>
@@ -2109,127 +2153,127 @@
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-    </row>
-    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="19" t="s">
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+    </row>
+    <row r="9" spans="1:10" ht="18.3" x14ac:dyDescent="0.7">
+      <c r="A9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="18" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18">
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="17">
         <v>22800</v>
       </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="18" t="s">
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="18" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7" t="s">
         <v>32</v>
       </c>
@@ -2237,58 +2281,78 @@
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
-      <c r="F15" s="18">
+      <c r="F15" s="17">
         <v>187</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="18">
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="17">
         <v>2</v>
       </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18" t="s">
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="F5:J5"/>
+  <mergeCells count="36">
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:J13"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="F6:J6"/>
     <mergeCell ref="B15:E15"/>
@@ -2301,20 +2365,18 @@
     <mergeCell ref="F7:J7"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="F8:J8"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:J17"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:J14"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="F5:J5"/>
   </mergeCells>
-  <dataValidations count="10">
+  <dataValidations count="11">
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Wan Interface" prompt="This is the WAN interface for our side of the tunnel and the input is case sensitive." sqref="B2:E2" xr:uid="{C07FD6AA-6C71-4C27-87CC-503A8E3B46BD}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Local CIDRS" prompt="These are the subnets or hosts included for our side of the tunnel. Enter in comma delimited format." sqref="B4:E4" xr:uid="{34119527-BAD6-49DE-A5C0-74EF2DF8CB35}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Peer Address" prompt="This is the public IP for our side of the tunnel." sqref="B5:E5" xr:uid="{C5D5A1BF-EB6B-4F8F-B69D-CA62D29A2644}"/>
@@ -2331,6 +2393,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Shared Key" prompt="Please input a private key to be used for the Phase 1 and Phase 2 if pfs is enabled." sqref="B11:E11" xr:uid="{72A00610-33B7-4187-B3A4-884D1FB4B0E4}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Peer ID" prompt="This is a unique 3 numeric character long Identifer for this tunnel.   " sqref="B15:E15" xr:uid="{D15BF637-3655-4D1A-A8C4-1B015D6EF7A7}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="LAN Interface" prompt="This is the LAN interface or interfaces for our side of the tunnel. Input is case sensitive." sqref="B3:E3" xr:uid="{E3189C81-B086-4599-B81D-D3C775E08099}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Tunnel Description" prompt="Comments are added to the tunnel interface. Useful for quick reminders of a tunnels purpose, or for recording information related to the tunnel." sqref="B18:E18" xr:uid="{11A1DB40-0F2A-4738-8A8B-B6494D047D80}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -2375,15 +2438,15 @@
       <selection activeCell="A2" sqref="A2:A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.41796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -2397,7 +2460,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="9" t="s">
         <v>38</v>
       </c>
@@ -2411,7 +2474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="9" t="s">
         <v>39</v>
       </c>
@@ -2425,7 +2488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="9" t="s">
         <v>41</v>
       </c>
@@ -2433,7 +2496,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="9" t="s">
         <v>42</v>
       </c>
@@ -2441,7 +2504,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="9" t="s">
         <v>43</v>
       </c>
@@ -2449,7 +2512,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="9" t="s">
         <v>44</v>
       </c>
@@ -2457,7 +2520,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="9" t="s">
         <v>45</v>
       </c>
@@ -2465,7 +2528,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="9" t="s">
         <v>46</v>
       </c>
@@ -2473,7 +2536,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="9" t="s">
         <v>47</v>
       </c>
@@ -2481,7 +2544,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="9" t="s">
         <v>48</v>
       </c>
@@ -2489,7 +2552,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="9" t="s">
         <v>49</v>
       </c>
@@ -2497,7 +2560,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="9" t="s">
         <v>50</v>
       </c>
@@ -2505,7 +2568,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="9" t="s">
         <v>51</v>
       </c>
@@ -2513,7 +2576,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="9" t="s">
         <v>52</v>
       </c>
@@ -2521,7 +2584,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="9" t="s">
         <v>53</v>
       </c>
@@ -2529,7 +2592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="9" t="s">
         <v>54</v>
       </c>
@@ -2537,7 +2600,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="9" t="s">
         <v>55</v>
       </c>
@@ -2545,42 +2608,42 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="9" t="s">
         <v>63</v>
       </c>
@@ -2607,12 +2670,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B6CAB0F47CC3754797586B7D92E57C5D" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="41d386b8d08e958c99720414287dc6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="27bdd63d-6ee8-4cd4-b819-860a9527756d" xmlns:ns3="891b5dd6-cc48-4739-b022-bf37421cabd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7e57c0ad5350a9654831ddf9bb92c513" ns2:_="" ns3:_="">
     <xsd:import namespace="27bdd63d-6ee8-4cd4-b819-860a9527756d"/>
@@ -2835,6 +2892,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2352FC38-A6D7-4700-A093-3B0BD301C6E7}">
   <ds:schemaRefs>
@@ -2844,15 +2907,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DB187FE-51AC-4561-AC8E-FAFC09F1C9C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F1C8CA7-7272-4C7C-89EE-4682936E3FAD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2869,4 +2923,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DB187FE-51AC-4561-AC8E-FAFC09F1C9C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: split p1 & p2 TTL for fortiwizard functions
</commit_message>
<xml_diff>
--- a/docs/AdminToolbox.FortiWizard/Examples/VPN Buildout Form.xlsx
+++ b/docs/AdminToolbox.FortiWizard/Examples/VPN Buildout Form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taylor\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA641F3-A49C-4970-B2A8-8FA421DFE456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E018DBC-5505-4C36-A4F7-4CBE6E9DE39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5549AC1C-0D2B-4CC9-98FF-5DC810AE9CED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5549AC1C-0D2B-4CC9-98FF-5DC810AE9CED}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="71">
   <si>
     <t>&lt;Company Name&gt; VPN Buildout Form</t>
   </si>
@@ -498,6 +498,9 @@
   </si>
   <si>
     <t>TTL Phase 2</t>
+  </si>
+  <si>
+    <t>Time To Live</t>
   </si>
 </sst>
 </file>
@@ -645,14 +648,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1097,7 +1100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467F2439-AFA4-4EB5-9722-C78966753CCE}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L1" sqref="L1:X1048576"/>
     </sheetView>
   </sheetViews>
@@ -1233,8 +1236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA6D4131-A607-49C7-BE92-430514422210}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,22 +1255,22 @@
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="16" t="s">
         <v>18</v>
       </c>
@@ -1280,10 +1283,10 @@
       <c r="A3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
       <c r="F3" s="16" t="s">
         <v>64</v>
       </c>
@@ -1296,10 +1299,10 @@
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="16" t="s">
         <v>19</v>
       </c>
@@ -1312,10 +1315,10 @@
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
       <c r="F5" s="16" t="s">
         <v>20</v>
       </c>
@@ -1328,10 +1331,10 @@
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
       <c r="F6" s="16" t="s">
         <v>25</v>
       </c>
@@ -1348,22 +1351,22 @@
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
       <c r="F8" s="16" t="s">
         <v>22</v>
       </c>
@@ -1376,10 +1379,10 @@
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
       <c r="F9" s="16" t="s">
         <v>23</v>
       </c>
@@ -1389,29 +1392,29 @@
       <c r="J9" s="16"/>
     </row>
     <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="17" t="s">
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="16" t="s">
         <v>65</v>
       </c>
@@ -1424,10 +1427,10 @@
       <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="16" t="s">
         <v>24</v>
       </c>
@@ -1440,10 +1443,10 @@
       <c r="A13" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
       <c r="F13" s="16">
         <v>86400</v>
       </c>
@@ -1456,10 +1459,10 @@
       <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
       <c r="F14" s="16" t="s">
         <v>26</v>
       </c>
@@ -1472,10 +1475,10 @@
       <c r="A15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
       <c r="F15" s="16" t="s">
         <v>30</v>
       </c>
@@ -1488,10 +1491,10 @@
       <c r="A16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
       <c r="F16" s="16">
         <v>2</v>
       </c>
@@ -1504,10 +1507,10 @@
       <c r="A17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
       <c r="F17" s="16" t="s">
         <v>34</v>
       </c>
@@ -1520,10 +1523,10 @@
       <c r="A18" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
       <c r="F18" s="16" t="s">
         <v>67</v>
       </c>
@@ -1536,10 +1539,10 @@
       <c r="A19" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
       <c r="F19" s="16">
         <v>22800</v>
       </c>
@@ -1550,14 +1553,20 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="F15:J15"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A7:E7"/>
@@ -1574,20 +1583,14 @@
     <mergeCell ref="F5:J5"/>
     <mergeCell ref="F6:J6"/>
     <mergeCell ref="F8:J8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F14:J14"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="F17:J17"/>
   </mergeCells>
   <dataValidations count="12">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Length" error="Tunnel Name must be less than 15 characters." promptTitle="Tunnel Name" prompt="This will be the name of the tunnel built on our Firewall. Must be less than 15 characters." sqref="B6:E6" xr:uid="{03F195E0-AFC6-4FC7-8F1F-7DE63D349659}">
@@ -1667,22 +1670,22 @@
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="16" t="s">
         <v>18</v>
       </c>
@@ -1695,10 +1698,10 @@
       <c r="A3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
       <c r="F3" s="16" t="s">
         <v>64</v>
       </c>
@@ -1711,10 +1714,10 @@
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="16" t="s">
         <v>19</v>
       </c>
@@ -1727,10 +1730,10 @@
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
       <c r="F5" s="16" t="s">
         <v>28</v>
       </c>
@@ -1743,10 +1746,10 @@
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
       <c r="F6" s="16" t="s">
         <v>20</v>
       </c>
@@ -1759,10 +1762,10 @@
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
       <c r="F7" s="16" t="s">
         <v>25</v>
       </c>
@@ -1779,22 +1782,22 @@
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
       <c r="F9" s="16" t="s">
         <v>22</v>
       </c>
@@ -1807,10 +1810,10 @@
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="16" t="s">
         <v>23</v>
       </c>
@@ -1820,29 +1823,29 @@
       <c r="J10" s="16"/>
     </row>
     <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="17" t="s">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="16" t="s">
         <v>65</v>
       </c>
@@ -1855,10 +1858,10 @@
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
       <c r="F13" s="16" t="s">
         <v>24</v>
       </c>
@@ -1871,10 +1874,10 @@
       <c r="A14" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
       <c r="F14" s="16">
         <v>86400</v>
       </c>
@@ -1887,10 +1890,10 @@
       <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
       <c r="F15" s="16" t="s">
         <v>26</v>
       </c>
@@ -1903,10 +1906,10 @@
       <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
       <c r="F16" s="16" t="s">
         <v>30</v>
       </c>
@@ -1919,10 +1922,10 @@
       <c r="A17" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
       <c r="F17" s="16">
         <v>2</v>
       </c>
@@ -1935,10 +1938,10 @@
       <c r="A18" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
       <c r="F18" s="16" t="s">
         <v>34</v>
       </c>
@@ -1951,10 +1954,10 @@
       <c r="A19" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
       <c r="F19" s="16" t="s">
         <v>67</v>
       </c>
@@ -1967,10 +1970,10 @@
       <c r="A20" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
       <c r="F20" s="16">
         <v>22800</v>
       </c>
@@ -1981,34 +1984,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="F20:J20"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:J17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:J14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:J9"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:J5"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="B2:E2"/>
@@ -2021,6 +1996,34 @@
     <mergeCell ref="F3:J3"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="F4:J4"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="F20:J20"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F18:J18"/>
   </mergeCells>
   <dataValidations count="13">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Local CIDRS" prompt="These are the NAT subnets or hosts included for our side of the tunnel. Enter in comma delimited format." sqref="B5:E5" xr:uid="{62A4F800-5137-4B7F-A2F4-0F3093E623BD}"/>
@@ -2082,10 +2085,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A920662-2A14-4585-A258-D7BC09CFE950}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B12" sqref="B12:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2102,22 +2105,22 @@
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="16" t="s">
         <v>18</v>
       </c>
@@ -2130,10 +2133,10 @@
       <c r="A3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
       <c r="F3" s="16" t="s">
         <v>64</v>
       </c>
@@ -2146,10 +2149,10 @@
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="16" t="s">
         <v>19</v>
       </c>
@@ -2162,10 +2165,10 @@
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
       <c r="F5" s="16" t="s">
         <v>20</v>
       </c>
@@ -2178,10 +2181,10 @@
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
       <c r="F6" s="16" t="s">
         <v>25</v>
       </c>
@@ -2198,22 +2201,22 @@
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
       <c r="F8" s="16" t="s">
         <v>22</v>
       </c>
@@ -2223,29 +2226,29 @@
       <c r="J8" s="16"/>
     </row>
     <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="17" t="s">
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="16" t="s">
         <v>65</v>
       </c>
@@ -2258,10 +2261,10 @@
       <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="16" t="s">
         <v>24</v>
       </c>
@@ -2272,12 +2275,12 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
+        <v>70</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="16">
         <v>86400</v>
       </c>
@@ -2290,10 +2293,10 @@
       <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
       <c r="F13" s="16" t="s">
         <v>26</v>
       </c>
@@ -2306,10 +2309,10 @@
       <c r="A14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
       <c r="F14" s="16" t="s">
         <v>30</v>
       </c>
@@ -2338,10 +2341,10 @@
       <c r="A16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
       <c r="F16" s="16">
         <v>2</v>
       </c>
@@ -2354,10 +2357,10 @@
       <c r="A17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
       <c r="F17" s="16" t="s">
         <v>34</v>
       </c>
@@ -2370,10 +2373,10 @@
       <c r="A18" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
       <c r="F18" s="16" t="s">
         <v>67</v>
       </c>
@@ -2382,36 +2385,18 @@
       <c r="I18" s="16"/>
       <c r="J18" s="16"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="16">
-        <v>22800</v>
-      </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-    </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:J17"/>
+  <mergeCells count="36">
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="F5:J5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="F6:J6"/>
     <mergeCell ref="B15:E15"/>
@@ -2428,18 +2413,18 @@
     <mergeCell ref="F11:J11"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="F14:J14"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:J17"/>
   </mergeCells>
-  <dataValidations count="12">
+  <dataValidations count="11">
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Wan Interface" prompt="This is the WAN interface for our side of the tunnel and the input is case sensitive." sqref="B2:E2" xr:uid="{C07FD6AA-6C71-4C27-87CC-503A8E3B46BD}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Local CIDRS" prompt="These are the subnets or hosts included for our side of the tunnel. Enter in comma delimited format." sqref="B4:E4" xr:uid="{34119527-BAD6-49DE-A5C0-74EF2DF8CB35}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Peer Address" prompt="This is the public IP for our side of the tunnel." sqref="B5:E5" xr:uid="{C5D5A1BF-EB6B-4F8F-B69D-CA62D29A2644}"/>
@@ -2453,11 +2438,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Peer ID" prompt="This is a unique 3 numeric character long Identifer for this tunnel.   " sqref="B15:E15" xr:uid="{D15BF637-3655-4D1A-A8C4-1B015D6EF7A7}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="LAN Interface" prompt="This is the LAN interface or interfaces for our side of the tunnel. Input is case sensitive." sqref="B3:E3" xr:uid="{E3189C81-B086-4599-B81D-D3C775E08099}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Tunnel Description" prompt="Comments are added to the tunnel interface. Useful for quick reminders of a tunnels purpose, or for recording information related to the tunnel. This is an optional field." sqref="B18:E18" xr:uid="{5A3E5F5C-84DD-4BE4-A087-8809DAC48E79}"/>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Valid range is 3600-86400. Please input a value in that range." promptTitle="TTL" prompt="This is the Phase 1 proposals time to live. Provide a value in the range of 3600-86400" sqref="B12:E12" xr:uid="{6062B940-31D2-47A5-A5F6-E80C1BCCBF85}">
-      <formula1>3600</formula1>
-      <formula2>86400</formula2>
-    </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Valid range is 3600-86400. Please input a value in that range." promptTitle="TTL" prompt="This is the Phase 2 proposals time to live. Provide a value in the range of 3600-86400" sqref="B19:E19" xr:uid="{9B668D06-8EDB-4EB1-8CA8-4080A69992B0}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Valid range is 3600-86400. Please input a value in that range." promptTitle="TTL" prompt="This is the Phase 2 proposals time to live. Phase 1 TTL is not provided for Dial Up tunnels. Provide a value in the range of 3600-86400" sqref="B12:E12" xr:uid="{6062B940-31D2-47A5-A5F6-E80C1BCCBF85}">
       <formula1>3600</formula1>
       <formula2>86400</formula2>
     </dataValidation>
@@ -2728,15 +2709,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B6CAB0F47CC3754797586B7D92E57C5D" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="41d386b8d08e958c99720414287dc6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="27bdd63d-6ee8-4cd4-b819-860a9527756d" xmlns:ns3="891b5dd6-cc48-4739-b022-bf37421cabd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7e57c0ad5350a9654831ddf9bb92c513" ns2:_="" ns3:_="">
     <xsd:import namespace="27bdd63d-6ee8-4cd4-b819-860a9527756d"/>
@@ -2959,6 +2931,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2966,14 +2947,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2352FC38-A6D7-4700-A093-3B0BD301C6E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F1C8CA7-7272-4C7C-89EE-4682936E3FAD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2992,6 +2965,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2352FC38-A6D7-4700-A093-3B0BD301C6E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DB187FE-51AC-4561-AC8E-FAFC09F1C9C9}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
feat: admintoolbox.fortiwizard add wildcard selectors
</commit_message>
<xml_diff>
--- a/docs/AdminToolbox.FortiWizard/Examples/VPN Buildout Form.xlsx
+++ b/docs/AdminToolbox.FortiWizard/Examples/VPN Buildout Form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taylor\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E018DBC-5505-4C36-A4F7-4CBE6E9DE39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CF3264-F1AB-4FA2-8D09-1AFF3C7D502C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5549AC1C-0D2B-4CC9-98FF-5DC810AE9CED}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{5549AC1C-0D2B-4CC9-98FF-5DC810AE9CED}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="72">
   <si>
     <t>&lt;Company Name&gt; VPN Buildout Form</t>
   </si>
@@ -501,6 +501,9 @@
   </si>
   <si>
     <t>Time To Live</t>
+  </si>
+  <si>
+    <t>Wildcard Selector</t>
   </si>
 </sst>
 </file>
@@ -612,7 +615,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -626,6 +629,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -648,14 +654,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -802,9 +808,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -842,7 +848,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -948,7 +954,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1090,7 +1096,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1107,111 +1113,111 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
     </row>
     <row r="2" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
       <c r="F6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
       <c r="F8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1234,363 +1240,380 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA6D4131-A607-49C7-BE92-430514422210}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="19" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="16" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="16" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="16" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="16" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="16" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="19" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="16" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="16" t="s">
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
     </row>
     <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="19" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="16" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="16" t="s">
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="16">
-        <v>86400</v>
-      </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
+        <v>69</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="17">
+        <v>22800</v>
+      </c>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
+        <v>68</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="17">
+        <v>86400</v>
+      </c>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
+        <v>16</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="16">
-        <v>2</v>
-      </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
+        <v>29</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
+        <v>32</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="17">
+        <v>2</v>
+      </c>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
+        <v>33</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="16">
-        <v>22800</v>
-      </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
+        <v>71</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="F14:J14"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="F12:J12"/>
+  <mergeCells count="39">
     <mergeCell ref="F13:J13"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="F20:J20"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="F8:J8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="F15:J15"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="F6:J6"/>
-    <mergeCell ref="F8:J8"/>
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="F9:J9"/>
   </mergeCells>
   <dataValidations count="12">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Length" error="Tunnel Name must be less than 15 characters." promptTitle="Tunnel Name" prompt="This will be the name of the tunnel built on our Firewall. Must be less than 15 characters." sqref="B6:E6" xr:uid="{03F195E0-AFC6-4FC7-8F1F-7DE63D349659}">
@@ -1603,22 +1626,22 @@
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Wan Interface" prompt="This is the WAN interface for our side of the tunnel and the input is case sensitive." sqref="B2:E2" xr:uid="{5B209772-0939-489C-9330-2A4A4C0FD6A4}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Subnets or Hosts" prompt="These are the subnets included for your side of the tunnel. Enter in comma delimited format as shown in the example." sqref="B8:E8" xr:uid="{F3FC9BFB-1638-4D1D-B294-12AA2CC89311}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Public IP" prompt="This is the public IP for your side of the tunnel." sqref="B9:E9" xr:uid="{90ECDB5C-D46F-431F-82F5-D71ABBC94518}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Leave Blank if All" prompt="These are the services that will be allowed for the tunnel. They should be provided in comma delimited format and typed like so… ServiceName/PortRange/Protocol" sqref="B15:E15" xr:uid="{A4A9A44A-13D1-4E58-9AC0-33A81A316D8B}"/>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Valid range is 3600-86400. Please input a value in that range." promptTitle="TTL" prompt="This is the Phase 2 proposals time to live. Provide a value in the range of 3600-86400" sqref="B19:E19" xr:uid="{08C633E1-0F6B-4D7A-876B-656FCCF5C8CC}">
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Leave Blank if All" prompt="These are the services that will be allowed for the tunnel. They should be provided in comma delimited format and typed like so… ServiceName/PortRange/Protocol" sqref="B16:E16" xr:uid="{A4A9A44A-13D1-4E58-9AC0-33A81A316D8B}"/>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Valid range is 3600-86400. Please input a value in that range." promptTitle="TTL" prompt="This is the Phase 2 proposals time to live. Provide a value in the range of 3600-86400" sqref="B13:E13" xr:uid="{08C633E1-0F6B-4D7A-876B-656FCCF5C8CC}">
       <formula1>3600</formula1>
       <formula2>86400</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Shared Key" prompt="Please input a private key to be used for the Phase 1 and Phase 2 if pfs is enabled." sqref="B12:E12" xr:uid="{9E459AD0-C2F6-47D4-82A2-D143255F65EC}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Tunnel Description" prompt="Comments are added to the tunnel interface. Useful for quick reminders of a tunnels purpose, or for recording information related to the tunnel. This is an optional field." sqref="B18:E18" xr:uid="{FD4C941C-BF15-4CE5-95BA-B14051345D75}"/>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Valid range is 3600-86400. Please input a value in that range." promptTitle="TTL" prompt="This is the Phase 1 proposals time to live. Provide a value in the range of 3600-86400" sqref="B13:E13" xr:uid="{B3CC6362-8A2C-40AE-8058-8D4C5C3F30FB}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Valid range is 3600-86400. Please input a value in that range." promptTitle="TTL" prompt="This is the Phase 1 proposals time to live. Provide a value in the range of 3600-86400" sqref="B14:E14" xr:uid="{B3CC6362-8A2C-40AE-8058-8D4C5C3F30FB}">
       <formula1>3600</formula1>
       <formula2>86400</formula2>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Tunnel Description" prompt="Comments are added to the tunnel interface. Useful for quick reminders of a tunnels purpose, or for recording information related to the tunnel. This is an optional field." sqref="B20:E20" xr:uid="{FD4C941C-BF15-4CE5-95BA-B14051345D75}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value Check" error="The value you entered doesn't match an option from the dropdown menu. Please use the drop down menu to select an option or ensure the format entered matches the example." promptTitle="Select an Option" prompt="Select a valid Phase 1 and Phase 2 proposal option from the drop down menu. If multiple values, they can be entered using the format shown in the example." xr:uid="{309CAFB7-A57D-4A82-9EF5-6DF84A1237ED}">
           <x14:formula1>
             <xm:f>'Data Validation'!$A$2:$A$26</xm:f>
@@ -1629,19 +1652,25 @@
           <x14:formula1>
             <xm:f>'Data Validation'!$C$2:$C$18</xm:f>
           </x14:formula1>
-          <xm:sqref>B14:E14</xm:sqref>
+          <xm:sqref>B15:E15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Select a valid option from the drop down list." promptTitle="Ike Version" prompt="This is the Ike version for the Phase 1 interface. Select a value from the drop down." xr:uid="{3BB213D7-7365-43CA-BB81-246CC40F55D9}">
           <x14:formula1>
             <xm:f>'Data Validation'!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B16:E16</xm:sqref>
+          <xm:sqref>B17:E17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Value" error="Select a valid value from the drop down list." promptTitle="Phase 2 PFS" prompt="This specifies if the phase 2 interface/s should have PFS enabled." xr:uid="{E4E22B61-9F00-4A61-9B2D-9613D5199D01}">
           <x14:formula1>
             <xm:f>'Data Validation'!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B17:E17</xm:sqref>
+          <xm:sqref>B18:E18</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Value" error="Select a valid value from the drop down list." promptTitle="Wildcard Selector" prompt="Specify if a wildcard selector should be used for the phase 2 or if phase 2 selectors should be paired off of remote and local CIDR addresses." xr:uid="{436A626B-8F82-4B3C-A25A-FC7869C5A3C1}">
+          <x14:formula1>
+            <xm:f>'Data Validation'!$E$2:$E$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B19:E19</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1651,339 +1680,385 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E09B223A-56BE-4F04-87ED-767E7017E672}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:J20"/>
+      <selection activeCell="A20" sqref="A20:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="19" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="16" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="16" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="16" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="16" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="16" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="16" t="s">
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
     </row>
     <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="19" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="16" t="s">
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="16" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
     </row>
     <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="19" t="s">
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="16" t="s">
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="16" t="s">
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="16">
-        <v>86400</v>
-      </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
+        <v>69</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="17">
+        <v>22800</v>
+      </c>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
+        <v>68</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="17">
+        <v>86400</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
+        <v>16</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="16">
-        <v>2</v>
-      </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
+        <v>29</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
+        <v>32</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="17">
+        <v>2</v>
+      </c>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
+        <v>33</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="16">
-        <v>22800</v>
-      </c>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
+        <v>71</v>
+      </c>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="41">
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="F21:J21"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:J5"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="B2:E2"/>
@@ -1996,34 +2071,6 @@
     <mergeCell ref="F3:J3"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="F4:J4"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:J9"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:J14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="F20:J20"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:J17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F18:J18"/>
   </mergeCells>
   <dataValidations count="13">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Local CIDRS" prompt="These are the NAT subnets or hosts included for our side of the tunnel. Enter in comma delimited format." sqref="B5:E5" xr:uid="{62A4F800-5137-4B7F-A2F4-0F3093E623BD}"/>
@@ -2036,15 +2083,15 @@
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Wan Interface" prompt="This is the WAN interface for our side of the tunnel and the input is case sensitive." sqref="B2:E2" xr:uid="{BA9BED3D-FC45-4642-99A7-C3D1037C4C1E}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Public IP" prompt="This is the public IP for your side of the tunnel." sqref="B10:E10" xr:uid="{E1D19247-04BB-4443-99DE-0A2763CE91C9}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Subnets or Hosts" prompt="These are the subnets included for your side of the tunnel. Enter in comma delimited format as shown in the example." sqref="B9:E9" xr:uid="{26978246-CC60-409C-8F88-3E819C638BC1}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Shared Key" prompt="Please input a private key to be used for the Phase 1 and Phase 2 if pfs is enabled." sqref="B13:E13" xr:uid="{B2E7618D-2434-482B-811B-D554973D35C1}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Leave Blank if All" prompt="These are the services that will be allowed for the tunnel. They should be provided in comma delimited format and typed like so… ServiceName/PortRange/Protocol" sqref="B16:E16" xr:uid="{2FFFEDB4-BC71-415C-9EF4-11B51AD3DDD8}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Shared Key" prompt="Please input a private key to be used for the Phase 1 and Phase 2 if pfs is enabled." sqref="B13:E14" xr:uid="{B2E7618D-2434-482B-811B-D554973D35C1}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Leave Blank if All" prompt="These are the services that will be allowed for the tunnel. They should be provided in comma delimited format and typed like so… ServiceName/PortRange/Protocol" sqref="B17:E17" xr:uid="{2FFFEDB4-BC71-415C-9EF4-11B51AD3DDD8}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="LAN Interface" prompt="This is the LAN interface or interfaces for our side of the tunnel. Input is case sensitive." sqref="B3:E3" xr:uid="{89AEF286-24FB-481D-9A83-43AFECCB6898}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Tunnel Description" prompt="Comments are added to the tunnel interface. Useful for quick reminders of a tunnels purpose, or for recording information related to the tunnel. This is an optional field." sqref="B19:E19" xr:uid="{D7AA2F75-80F6-4FBF-A84F-1B5797CD4C8B}"/>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Valid range is 3600-86400. Please input a value in that range." promptTitle="TTL" prompt="This is the Phase 1 proposals time to live. Provide a value in the range of 3600-86400" sqref="B14:E14" xr:uid="{3D044945-ED11-46D0-82BC-A1647E6D3222}">
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Tunnel Description" prompt="Comments are added to the tunnel interface. Useful for quick reminders of a tunnels purpose, or for recording information related to the tunnel. This is an optional field." sqref="B21:E21" xr:uid="{D7AA2F75-80F6-4FBF-A84F-1B5797CD4C8B}"/>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Valid range is 3600-86400. Please input a value in that range." promptTitle="TTL" prompt="This is the Phase 1 proposals time to live. Provide a value in the range of 3600-86400" sqref="B15:E15" xr:uid="{3D044945-ED11-46D0-82BC-A1647E6D3222}">
       <formula1>3600</formula1>
       <formula2>86400</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Valid range is 3600-86400. Please input a value in that range." promptTitle="TTL" prompt="This is the Phase 2 proposals time to live. Provide a value in the range of 3600-86400" sqref="B20:E20" xr:uid="{FD831958-ABAF-4D6D-A5CC-6B017CC93478}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Valid range is 3600-86400. Please input a value in that range." promptTitle="TTL" prompt="This is the Phase 2 proposals time to live. Provide a value in the range of 3600-86400" sqref="B14:E14" xr:uid="{FD831958-ABAF-4D6D-A5CC-6B017CC93478}">
       <formula1>3600</formula1>
       <formula2>86400</formula2>
     </dataValidation>
@@ -2052,30 +2099,36 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Value" error="Select a valid value from the drop down list." promptTitle="Phase 2 PFS" prompt="This specifies if the phase 2 interface/s should have PFS enabled." xr:uid="{60EAC752-411F-4170-A2B1-B2F2864C94C4}">
           <x14:formula1>
             <xm:f>'Data Validation'!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B18:E18</xm:sqref>
+          <xm:sqref>B19:E19</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Select a valid option from the drop down list." promptTitle="Ike Version" prompt="This is the Ike version for the Phase 1 interface. Select a value from the drop down." xr:uid="{6393646A-0F9C-448E-B1EE-130EEF04CA51}">
           <x14:formula1>
             <xm:f>'Data Validation'!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B17:E17</xm:sqref>
+          <xm:sqref>B18:E18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value Check" error="The value you entered doesn't match an option from the dropdown menu. Please correct or continue if your value matches the format shown in the example." promptTitle="Select an Option" prompt="Select a valid Diffie Hellman Group from the drop down menu, or type your own comma delimited option. Like what is shown in the example." xr:uid="{5A743148-89D6-4C6F-99C3-80048B1848E8}">
           <x14:formula1>
             <xm:f>'Data Validation'!$C$2:$C$18</xm:f>
           </x14:formula1>
-          <xm:sqref>B15:E15</xm:sqref>
+          <xm:sqref>B16:E16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value Check" error="The value you entered doesn't match an option from the dropdown menu. Please use the drop down menu to select an option or ensure the format entered matches the example." promptTitle="Select an Option" prompt="Select a valid Phase 1 and Phase 2 proposal option from the drop down menu. If multiple values, they can be entered using the format shown in the example." xr:uid="{5CC1424D-68FD-4BAB-865B-3F69AC0D8E5E}">
           <x14:formula1>
             <xm:f>'Data Validation'!$A$2:$A$26</xm:f>
           </x14:formula1>
           <xm:sqref>B12:E12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Value" error="Select a valid value from the drop down list." promptTitle="Wildcard Selector" prompt="Specify if a wildcard selector should be used for the phase 2 or if phase 2 selectors should be paired off of remote and local CIDR addresses." xr:uid="{E506124B-92DC-44F5-8E7C-82762A0C6373}">
+          <x14:formula1>
+            <xm:f>'Data Validation'!$E$2:$E$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B20:E20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2085,10 +2138,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A920662-2A14-4585-A258-D7BC09CFE950}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2098,305 +2151,322 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="19" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="16" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="16" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="16" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="16" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="16" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="19" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="16" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
     </row>
     <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="19" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="16" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="16" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="16">
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="17">
         <v>86400</v>
       </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="16" t="s">
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="16" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="16">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="17">
         <v>187</v>
       </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="16">
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="17">
         <v>2</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="16" t="s">
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="16" t="s">
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="F5:J5"/>
+  <mergeCells count="37">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="B18:E18"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="F6:J6"/>
     <mergeCell ref="B15:E15"/>
@@ -2413,16 +2483,16 @@
     <mergeCell ref="F11:J11"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="F14:J14"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="F5:J5"/>
   </mergeCells>
   <dataValidations count="11">
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Wan Interface" prompt="This is the WAN interface for our side of the tunnel and the input is case sensitive." sqref="B2:E2" xr:uid="{C07FD6AA-6C71-4C27-87CC-503A8E3B46BD}"/>
@@ -2437,7 +2507,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Shared Key" prompt="Please input a private key to be used for the Phase 1 and Phase 2 if pfs is enabled." sqref="B11:E11" xr:uid="{72A00610-33B7-4187-B3A4-884D1FB4B0E4}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Peer ID" prompt="This is a unique 3 numeric character long Identifer for this tunnel.   " sqref="B15:E15" xr:uid="{D15BF637-3655-4D1A-A8C4-1B015D6EF7A7}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="LAN Interface" prompt="This is the LAN interface or interfaces for our side of the tunnel. Input is case sensitive." sqref="B3:E3" xr:uid="{E3189C81-B086-4599-B81D-D3C775E08099}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Tunnel Description" prompt="Comments are added to the tunnel interface. Useful for quick reminders of a tunnels purpose, or for recording information related to the tunnel. This is an optional field." sqref="B18:E18" xr:uid="{5A3E5F5C-84DD-4BE4-A087-8809DAC48E79}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Tunnel Description" prompt="Comments are added to the tunnel interface. Useful for quick reminders of a tunnels purpose, or for recording information related to the tunnel. This is an optional field." sqref="B19:E19" xr:uid="{5A3E5F5C-84DD-4BE4-A087-8809DAC48E79}"/>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Valid range is 3600-86400. Please input a value in that range." promptTitle="TTL" prompt="This is the Phase 2 proposals time to live. Phase 1 TTL is not provided for Dial Up tunnels. Provide a value in the range of 3600-86400" sqref="B12:E12" xr:uid="{6062B940-31D2-47A5-A5F6-E80C1BCCBF85}">
       <formula1>3600</formula1>
       <formula2>86400</formula2>
@@ -2447,7 +2517,7 @@
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value Check" error="The value you entered doesn't match an option from the dropdown menu. Please correct or continue if your value matches the format shown in the example." promptTitle="Select an Option" prompt="Select a valid Diffie Hellman Group from the drop down menu, or type your own comma delimited option. Like what is shown in the example." xr:uid="{6FEE91C3-ABD3-43A0-8E18-2C7C180C143B}">
           <x14:formula1>
             <xm:f>'Data Validation'!$C$2:$C$18</xm:f>
@@ -2471,6 +2541,12 @@
             <xm:f>'Data Validation'!$A$2:$A$26</xm:f>
           </x14:formula1>
           <xm:sqref>B10:E10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Value" error="Select a valid value from the drop down list." promptTitle="Wildcard Selector" prompt="Specify if a wildcard selector should be used for the phase 2 or if phase 2 selectors should be paired off of remote and local CIDR addresses." xr:uid="{73D7F5C7-54E3-4E67-9906-A1880B9ADE62}">
+          <x14:formula1>
+            <xm:f>'Data Validation'!$E$2:$E$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B18:E18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2709,6 +2785,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B6CAB0F47CC3754797586B7D92E57C5D" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="41d386b8d08e958c99720414287dc6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="27bdd63d-6ee8-4cd4-b819-860a9527756d" xmlns:ns3="891b5dd6-cc48-4739-b022-bf37421cabd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7e57c0ad5350a9654831ddf9bb92c513" ns2:_="" ns3:_="">
     <xsd:import namespace="27bdd63d-6ee8-4cd4-b819-860a9527756d"/>
@@ -2931,22 +3022,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DB187FE-51AC-4561-AC8E-FAFC09F1C9C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2352FC38-A6D7-4700-A093-3B0BD301C6E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F1C8CA7-7272-4C7C-89EE-4682936E3FAD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2963,21 +3056,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2352FC38-A6D7-4700-A093-3B0BD301C6E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DB187FE-51AC-4561-AC8E-FAFC09F1C9C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>